<commit_message>
New plots including modeling parameters
</commit_message>
<xml_diff>
--- a/data_sum/operant_sample1_modeling.xlsx
+++ b/data_sum/operant_sample1_modeling.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/larawieland/Documents/Promotion/SALAD/data_sum/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4259BA1A-5C33-524F-88AB-8DDC6827E5F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1E391A5-89F2-3F4D-A4D5-AF8526A859C0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9520" yWindow="1640" windowWidth="24340" windowHeight="14780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2040" yWindow="660" windowWidth="24340" windowHeight="14780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1552" uniqueCount="1147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1558" uniqueCount="1153">
   <si>
     <t>sub_id</t>
   </si>
@@ -3461,16 +3461,40 @@
   </si>
   <si>
     <t>BIS_total</t>
+  </si>
+  <si>
+    <t>log_lik</t>
+  </si>
+  <si>
+    <t>al_win</t>
+  </si>
+  <si>
+    <t>kappa</t>
+  </si>
+  <si>
+    <t>al_loss</t>
+  </si>
+  <si>
+    <t>beta_win</t>
+  </si>
+  <si>
+    <t>beta_loss</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -3516,9 +3540,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A1:BP29" totalsRowShown="0">
-  <autoFilter ref="A1:BP29" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
-  <tableColumns count="68">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A1:BV29" totalsRowShown="0">
+  <autoFilter ref="A1:BV29" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+  <tableColumns count="74">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="sub_id"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="group"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="order"/>
@@ -3587,6 +3611,12 @@
     <tableColumn id="65" xr3:uid="{00000000-0010-0000-0000-000041000000}" name="p_l_sw_pre_T2"/>
     <tableColumn id="66" xr3:uid="{00000000-0010-0000-0000-000042000000}" name="p_l_sw_rev_T2"/>
     <tableColumn id="67" xr3:uid="{00000000-0010-0000-0000-000043000000}" name="p_l_sw_post_T2"/>
+    <tableColumn id="69" xr3:uid="{C9E64459-163E-9A4A-9165-7E8C66BCCE69}" name="log_lik"/>
+    <tableColumn id="70" xr3:uid="{BAE2B17A-025A-8D49-9760-390887D490A7}" name="al_win"/>
+    <tableColumn id="71" xr3:uid="{5621703F-F3CE-FF41-9D43-A6AE312C432B}" name="al_loss"/>
+    <tableColumn id="72" xr3:uid="{0B293E2D-F95A-5141-87D7-395B202440AB}" name="kappa"/>
+    <tableColumn id="73" xr3:uid="{79E7B7CC-4CBC-4C48-9548-EBE9CF1427DB}" name="beta_win"/>
+    <tableColumn id="74" xr3:uid="{256345A5-776B-0342-A9BF-B089C9C050C1}" name="beta_loss"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3871,15 +3901,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BP29"/>
+  <dimension ref="A1:BV29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L33" sqref="L33"/>
+    <sheetView tabSelected="1" topLeftCell="BI1" workbookViewId="0">
+      <selection activeCell="BO11" sqref="BO11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:68" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4084,8 +4114,26 @@
       <c r="BP1" t="s">
         <v>66</v>
       </c>
+      <c r="BQ1" t="s">
+        <v>1147</v>
+      </c>
+      <c r="BR1" t="s">
+        <v>1148</v>
+      </c>
+      <c r="BS1" t="s">
+        <v>1150</v>
+      </c>
+      <c r="BT1" t="s">
+        <v>1149</v>
+      </c>
+      <c r="BU1" t="s">
+        <v>1151</v>
+      </c>
+      <c r="BV1" t="s">
+        <v>1152</v>
+      </c>
     </row>
-    <row r="2" spans="1:68" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>67</v>
       </c>
@@ -4290,8 +4338,26 @@
       <c r="BP2" t="s">
         <v>119</v>
       </c>
+      <c r="BQ2">
+        <v>-195.24523001490601</v>
+      </c>
+      <c r="BR2">
+        <v>0.27650000000000002</v>
+      </c>
+      <c r="BS2">
+        <v>0.74339999999999995</v>
+      </c>
+      <c r="BT2">
+        <v>-0.59751766350473201</v>
+      </c>
+      <c r="BU2">
+        <v>0.70918673554329703</v>
+      </c>
+      <c r="BV2">
+        <v>-0.42291431385054601</v>
+      </c>
     </row>
-    <row r="3" spans="1:68" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>120</v>
       </c>
@@ -4496,8 +4562,26 @@
       <c r="BP3" t="s">
         <v>101</v>
       </c>
+      <c r="BQ3">
+        <v>-165.26080230379301</v>
+      </c>
+      <c r="BR3">
+        <v>0.32290000000000002</v>
+      </c>
+      <c r="BS3">
+        <v>0.88219999999999998</v>
+      </c>
+      <c r="BT3">
+        <v>-0.33299572561956597</v>
+      </c>
+      <c r="BU3">
+        <v>1.02957655196939</v>
+      </c>
+      <c r="BV3">
+        <v>0.46879038000710099</v>
+      </c>
     </row>
-    <row r="4" spans="1:68" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>166</v>
       </c>
@@ -4702,8 +4786,26 @@
       <c r="BP4" t="s">
         <v>213</v>
       </c>
+      <c r="BQ4">
+        <v>-101.47496579892901</v>
+      </c>
+      <c r="BR4">
+        <v>0.23</v>
+      </c>
+      <c r="BS4">
+        <v>0.92769999999999997</v>
+      </c>
+      <c r="BT4">
+        <v>-1.76299798096754</v>
+      </c>
+      <c r="BU4">
+        <v>1.70106939969715</v>
+      </c>
+      <c r="BV4">
+        <v>1.3525657350028</v>
+      </c>
     </row>
-    <row r="5" spans="1:68" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>214</v>
       </c>
@@ -4908,8 +5010,26 @@
       <c r="BP5" t="s">
         <v>213</v>
       </c>
+      <c r="BQ5">
+        <v>-65.755395678022396</v>
+      </c>
+      <c r="BR5">
+        <v>0.21859999999999999</v>
+      </c>
+      <c r="BS5">
+        <v>0.61099999999999999</v>
+      </c>
+      <c r="BT5">
+        <v>-0.99090813395190702</v>
+      </c>
+      <c r="BU5">
+        <v>2.01221574468331</v>
+      </c>
+      <c r="BV5">
+        <v>1.4327477919953999</v>
+      </c>
     </row>
-    <row r="6" spans="1:68" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>261</v>
       </c>
@@ -5114,8 +5234,26 @@
       <c r="BP6" t="s">
         <v>305</v>
       </c>
+      <c r="BQ6">
+        <v>-193.48568947408901</v>
+      </c>
+      <c r="BR6">
+        <v>0.24859999999999999</v>
+      </c>
+      <c r="BS6">
+        <v>0.92749999999999999</v>
+      </c>
+      <c r="BT6">
+        <v>-0.29302557277204</v>
+      </c>
+      <c r="BU6">
+        <v>0.645611501496689</v>
+      </c>
+      <c r="BV6">
+        <v>0.45243428769427402</v>
+      </c>
     </row>
-    <row r="7" spans="1:68" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>306</v>
       </c>
@@ -5320,8 +5458,26 @@
       <c r="BP7" t="s">
         <v>312</v>
       </c>
+      <c r="BQ7">
+        <v>-113.570517310347</v>
+      </c>
+      <c r="BR7">
+        <v>0.2039</v>
+      </c>
+      <c r="BS7">
+        <v>0.49730000000000002</v>
+      </c>
+      <c r="BT7">
+        <v>-0.95623048809300604</v>
+      </c>
+      <c r="BU7">
+        <v>1.6559707678286</v>
+      </c>
+      <c r="BV7">
+        <v>1.6041850537107101</v>
+      </c>
     </row>
-    <row r="8" spans="1:68" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>349</v>
       </c>
@@ -5523,8 +5679,26 @@
       <c r="BP8" t="s">
         <v>213</v>
       </c>
+      <c r="BQ8">
+        <v>-81.0274810010431</v>
+      </c>
+      <c r="BR8">
+        <v>0.29530000000000001</v>
+      </c>
+      <c r="BS8">
+        <v>0.76160000000000005</v>
+      </c>
+      <c r="BT8">
+        <v>-1.22511215610414</v>
+      </c>
+      <c r="BU8">
+        <v>1.8751071144323701</v>
+      </c>
+      <c r="BV8">
+        <v>1.3270453347473901</v>
+      </c>
     </row>
-    <row r="9" spans="1:68" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>395</v>
       </c>
@@ -5729,8 +5903,26 @@
       <c r="BP9" t="s">
         <v>437</v>
       </c>
+      <c r="BQ9">
+        <v>-153.28737607999301</v>
+      </c>
+      <c r="BR9">
+        <v>0.37509999999999999</v>
+      </c>
+      <c r="BS9">
+        <v>0.87639999999999996</v>
+      </c>
+      <c r="BT9">
+        <v>0.155182060518574</v>
+      </c>
+      <c r="BU9">
+        <v>1.0768682501890099</v>
+      </c>
+      <c r="BV9">
+        <v>5.0772242594244003E-2</v>
+      </c>
     </row>
-    <row r="10" spans="1:68" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>438</v>
       </c>
@@ -5935,8 +6127,26 @@
       <c r="BP10" t="s">
         <v>213</v>
       </c>
+      <c r="BQ10">
+        <v>-36.2772334443777</v>
+      </c>
+      <c r="BR10">
+        <v>0.1147</v>
+      </c>
+      <c r="BS10">
+        <v>0.6784</v>
+      </c>
+      <c r="BT10">
+        <v>-3.4697156398402198</v>
+      </c>
+      <c r="BU10">
+        <v>2.7614574858654</v>
+      </c>
+      <c r="BV10">
+        <v>2.3663676394868398</v>
+      </c>
     </row>
-    <row r="11" spans="1:68" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>462</v>
       </c>
@@ -6138,8 +6348,26 @@
       <c r="BP11" t="s">
         <v>334</v>
       </c>
+      <c r="BQ11">
+        <v>-176.20970671031299</v>
+      </c>
+      <c r="BR11">
+        <v>0.30130000000000001</v>
+      </c>
+      <c r="BS11">
+        <v>0.79469999999999996</v>
+      </c>
+      <c r="BT11">
+        <v>-2.2695774014510102</v>
+      </c>
+      <c r="BU11">
+        <v>0.91615615799420203</v>
+      </c>
+      <c r="BV11">
+        <v>0.72365446505258002</v>
+      </c>
     </row>
-    <row r="12" spans="1:68" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>503</v>
       </c>
@@ -6344,8 +6572,26 @@
       <c r="BP12" t="s">
         <v>547</v>
       </c>
+      <c r="BQ12">
+        <v>-129.59821727707401</v>
+      </c>
+      <c r="BR12">
+        <v>0.47770000000000001</v>
+      </c>
+      <c r="BS12">
+        <v>0.90669999999999995</v>
+      </c>
+      <c r="BT12">
+        <v>-0.31101176545220599</v>
+      </c>
+      <c r="BU12">
+        <v>1.1192423119757899</v>
+      </c>
+      <c r="BV12">
+        <v>1.03779990004914</v>
+      </c>
     </row>
-    <row r="13" spans="1:68" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>548</v>
       </c>
@@ -6550,8 +6796,26 @@
       <c r="BP13" t="s">
         <v>213</v>
       </c>
+      <c r="BQ13">
+        <v>-60.571385672718101</v>
+      </c>
+      <c r="BR13">
+        <v>0.31480000000000002</v>
+      </c>
+      <c r="BS13">
+        <v>0.61270000000000002</v>
+      </c>
+      <c r="BT13">
+        <v>-1.32791011237045</v>
+      </c>
+      <c r="BU13">
+        <v>2.0580095457991399</v>
+      </c>
+      <c r="BV13">
+        <v>1.43560488757254</v>
+      </c>
     </row>
-    <row r="14" spans="1:68" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>587</v>
       </c>
@@ -6756,8 +7020,26 @@
       <c r="BP14" t="s">
         <v>213</v>
       </c>
+      <c r="BQ14">
+        <v>-94.976580414405802</v>
+      </c>
+      <c r="BR14">
+        <v>0.42920000000000003</v>
+      </c>
+      <c r="BS14">
+        <v>0.92079999999999995</v>
+      </c>
+      <c r="BT14">
+        <v>-0.43466934283172798</v>
+      </c>
+      <c r="BU14">
+        <v>1.5280735742400799</v>
+      </c>
+      <c r="BV14">
+        <v>0.80703860568608998</v>
+      </c>
     </row>
-    <row r="15" spans="1:68" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>623</v>
       </c>
@@ -6962,8 +7244,26 @@
       <c r="BP15" t="s">
         <v>661</v>
       </c>
+      <c r="BQ15">
+        <v>-105.125024479212</v>
+      </c>
+      <c r="BR15">
+        <v>0.41760000000000003</v>
+      </c>
+      <c r="BS15">
+        <v>0.82040000000000002</v>
+      </c>
+      <c r="BT15">
+        <v>-0.73835003836202995</v>
+      </c>
+      <c r="BU15">
+        <v>1.6033147288251199</v>
+      </c>
+      <c r="BV15">
+        <v>8.2613650931698895E-2</v>
+      </c>
     </row>
-    <row r="16" spans="1:68" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>662</v>
       </c>
@@ -7168,8 +7468,26 @@
       <c r="BP16" t="s">
         <v>213</v>
       </c>
+      <c r="BQ16">
+        <v>-57.811669798091401</v>
+      </c>
+      <c r="BR16">
+        <v>0.30570000000000003</v>
+      </c>
+      <c r="BS16">
+        <v>0.76500000000000001</v>
+      </c>
+      <c r="BT16">
+        <v>-1.47391208041934</v>
+      </c>
+      <c r="BU16">
+        <v>2.09398730181656</v>
+      </c>
+      <c r="BV16">
+        <v>1.75676989537803</v>
+      </c>
     </row>
-    <row r="17" spans="1:68" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>693</v>
       </c>
@@ -7374,8 +7692,26 @@
       <c r="BP17" t="s">
         <v>245</v>
       </c>
+      <c r="BQ17">
+        <v>-115.194053235957</v>
+      </c>
+      <c r="BR17">
+        <v>0.26200000000000001</v>
+      </c>
+      <c r="BS17">
+        <v>0.82210000000000005</v>
+      </c>
+      <c r="BT17">
+        <v>-1.0707873426015899</v>
+      </c>
+      <c r="BU17">
+        <v>1.5906079169978899</v>
+      </c>
+      <c r="BV17">
+        <v>0.69118923646263297</v>
+      </c>
     </row>
-    <row r="18" spans="1:68" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>728</v>
       </c>
@@ -7577,8 +7913,26 @@
       <c r="BP18" t="s">
         <v>126</v>
       </c>
+      <c r="BQ18">
+        <v>-100.150514235363</v>
+      </c>
+      <c r="BR18">
+        <v>0.31340000000000001</v>
+      </c>
+      <c r="BS18">
+        <v>0.89759999999999995</v>
+      </c>
+      <c r="BT18">
+        <v>0.369544565129868</v>
+      </c>
+      <c r="BU18">
+        <v>1.5011309256635199</v>
+      </c>
+      <c r="BV18">
+        <v>0.99966629456970302</v>
+      </c>
     </row>
-    <row r="19" spans="1:68" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>762</v>
       </c>
@@ -7780,8 +8134,26 @@
       <c r="BP19" t="s">
         <v>101</v>
       </c>
+      <c r="BQ19">
+        <v>-176.71758865828599</v>
+      </c>
+      <c r="BR19">
+        <v>0.1067</v>
+      </c>
+      <c r="BS19">
+        <v>0.72709999999999997</v>
+      </c>
+      <c r="BT19">
+        <v>-1.2759578059546901</v>
+      </c>
+      <c r="BU19">
+        <v>1.4511630742980901</v>
+      </c>
+      <c r="BV19">
+        <v>-5.4760836326000199E-2</v>
+      </c>
     </row>
-    <row r="20" spans="1:68" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>800</v>
       </c>
@@ -7986,8 +8358,26 @@
       <c r="BP20" t="s">
         <v>836</v>
       </c>
+      <c r="BQ20">
+        <v>-101.67088325247801</v>
+      </c>
+      <c r="BR20">
+        <v>0.317</v>
+      </c>
+      <c r="BS20">
+        <v>0.81130000000000002</v>
+      </c>
+      <c r="BT20">
+        <v>-0.54412988590080202</v>
+      </c>
+      <c r="BU20">
+        <v>1.7790091285483101</v>
+      </c>
+      <c r="BV20">
+        <v>1.12841757442276</v>
+      </c>
     </row>
-    <row r="21" spans="1:68" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>837</v>
       </c>
@@ -8192,8 +8582,26 @@
       <c r="BP21" t="s">
         <v>99</v>
       </c>
+      <c r="BQ21">
+        <v>-134.796221624216</v>
+      </c>
+      <c r="BR21">
+        <v>0.36940000000000001</v>
+      </c>
+      <c r="BS21">
+        <v>0.89710000000000001</v>
+      </c>
+      <c r="BT21">
+        <v>-1.1831840361529</v>
+      </c>
+      <c r="BU21">
+        <v>1.3234407918386299</v>
+      </c>
+      <c r="BV21">
+        <v>0.482531567602069</v>
+      </c>
     </row>
-    <row r="22" spans="1:68" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>875</v>
       </c>
@@ -8398,8 +8806,26 @@
       <c r="BP22" t="s">
         <v>196</v>
       </c>
+      <c r="BQ22">
+        <v>-98.593096553727406</v>
+      </c>
+      <c r="BR22">
+        <v>0.26889999999999997</v>
+      </c>
+      <c r="BS22">
+        <v>0.87370000000000003</v>
+      </c>
+      <c r="BT22">
+        <v>-1.2795619426334099</v>
+      </c>
+      <c r="BU22">
+        <v>1.8796881403993599</v>
+      </c>
+      <c r="BV22">
+        <v>0.82152876434571698</v>
+      </c>
     </row>
-    <row r="23" spans="1:68" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>911</v>
       </c>
@@ -8604,8 +9030,26 @@
       <c r="BP23" t="s">
         <v>213</v>
       </c>
+      <c r="BQ23">
+        <v>-117.579142180875</v>
+      </c>
+      <c r="BR23">
+        <v>0.32040000000000002</v>
+      </c>
+      <c r="BS23">
+        <v>0.86150000000000004</v>
+      </c>
+      <c r="BT23">
+        <v>-0.71704458688894102</v>
+      </c>
+      <c r="BU23">
+        <v>1.4631170900794599</v>
+      </c>
+      <c r="BV23">
+        <v>1.08708767510257</v>
+      </c>
     </row>
-    <row r="24" spans="1:68" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>946</v>
       </c>
@@ -8810,8 +9254,26 @@
       <c r="BP24" t="s">
         <v>330</v>
       </c>
+      <c r="BQ24">
+        <v>-162.18186632209</v>
+      </c>
+      <c r="BR24">
+        <v>0.12759999999999999</v>
+      </c>
+      <c r="BS24">
+        <v>0.25459999999999999</v>
+      </c>
+      <c r="BT24">
+        <v>-2.0520179673243502</v>
+      </c>
+      <c r="BU24">
+        <v>1.5873608032834201</v>
+      </c>
+      <c r="BV24">
+        <v>0.96186727280885898</v>
+      </c>
     </row>
-    <row r="25" spans="1:68" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>982</v>
       </c>
@@ -9016,8 +9478,26 @@
       <c r="BP25" t="s">
         <v>95</v>
       </c>
+      <c r="BQ25">
+        <v>-58.184112111257299</v>
+      </c>
+      <c r="BR25">
+        <v>0.30249999999999999</v>
+      </c>
+      <c r="BS25">
+        <v>0.50680000000000003</v>
+      </c>
+      <c r="BT25">
+        <v>-1.0714361175579501</v>
+      </c>
+      <c r="BU25">
+        <v>1.8317257290739599</v>
+      </c>
+      <c r="BV25">
+        <v>1.8052383920493</v>
+      </c>
     </row>
-    <row r="26" spans="1:68" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>1011</v>
       </c>
@@ -9222,8 +9702,26 @@
       <c r="BP26" t="s">
         <v>713</v>
       </c>
+      <c r="BQ26">
+        <v>-75.349284475398306</v>
+      </c>
+      <c r="BR26">
+        <v>0.33450000000000002</v>
+      </c>
+      <c r="BS26">
+        <v>0.32969999999999999</v>
+      </c>
+      <c r="BT26">
+        <v>-1.5480920879250499</v>
+      </c>
+      <c r="BU26">
+        <v>1.71137806116449</v>
+      </c>
+      <c r="BV26">
+        <v>2.2558751583223802</v>
+      </c>
     </row>
-    <row r="27" spans="1:68" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>1051</v>
       </c>
@@ -9428,8 +9926,26 @@
       <c r="BP27" t="s">
         <v>843</v>
       </c>
+      <c r="BQ27">
+        <v>-114.67111241329999</v>
+      </c>
+      <c r="BR27">
+        <v>0.32540000000000002</v>
+      </c>
+      <c r="BS27">
+        <v>0.89729999999999999</v>
+      </c>
+      <c r="BT27">
+        <v>-0.81103065015539</v>
+      </c>
+      <c r="BU27">
+        <v>1.70783692537763</v>
+      </c>
+      <c r="BV27">
+        <v>-0.125085432174869</v>
+      </c>
     </row>
-    <row r="28" spans="1:68" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>1085</v>
       </c>
@@ -9634,8 +10150,26 @@
       <c r="BP28" t="s">
         <v>126</v>
       </c>
+      <c r="BQ28">
+        <v>-49.3868939940239</v>
+      </c>
+      <c r="BR28">
+        <v>0.27060000000000001</v>
+      </c>
+      <c r="BS28">
+        <v>0.72709999999999997</v>
+      </c>
+      <c r="BT28">
+        <v>-2.0177914044123502</v>
+      </c>
+      <c r="BU28">
+        <v>2.4039996018230299</v>
+      </c>
+      <c r="BV28">
+        <v>1.8365387948684899</v>
+      </c>
     </row>
-    <row r="29" spans="1:68" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>1110</v>
       </c>
@@ -9840,8 +10374,27 @@
       <c r="BP29" t="s">
         <v>647</v>
       </c>
+      <c r="BQ29">
+        <v>-82.294699015430794</v>
+      </c>
+      <c r="BR29">
+        <v>0.19639999999999999</v>
+      </c>
+      <c r="BS29">
+        <v>0.23749999999999999</v>
+      </c>
+      <c r="BT29">
+        <v>-0.36222088391919599</v>
+      </c>
+      <c r="BU29">
+        <v>1.96481284620143</v>
+      </c>
+      <c r="BV29">
+        <v>1.6009380656563701</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Added params from best model to data file and some modeling plots
</commit_message>
<xml_diff>
--- a/data_sum/operant_sample1_modeling.xlsx
+++ b/data_sum/operant_sample1_modeling.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/larawieland/Documents/Promotion/SALAD/data_sum/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/larawieland/Documents/Promotion/SALAD_3/data_sum/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1E391A5-89F2-3F4D-A4D5-AF8526A859C0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB6F32B0-CFCA-1049-B381-72E86897F3F3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2040" yWindow="660" windowWidth="24340" windowHeight="14780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3463,22 +3463,22 @@
     <t>BIS_total</t>
   </si>
   <si>
-    <t>log_lik</t>
-  </si>
-  <si>
     <t>al_win</t>
   </si>
   <si>
-    <t>kappa</t>
-  </si>
-  <si>
     <t>al_loss</t>
   </si>
   <si>
-    <t>beta_win</t>
-  </si>
-  <si>
-    <t>beta_loss</t>
+    <t>bet_win</t>
+  </si>
+  <si>
+    <t>bet_loss</t>
+  </si>
+  <si>
+    <t>sc_bet_win</t>
+  </si>
+  <si>
+    <t>sc_bet_loss</t>
   </si>
 </sst>
 </file>
@@ -3611,12 +3611,12 @@
     <tableColumn id="65" xr3:uid="{00000000-0010-0000-0000-000041000000}" name="p_l_sw_pre_T2"/>
     <tableColumn id="66" xr3:uid="{00000000-0010-0000-0000-000042000000}" name="p_l_sw_rev_T2"/>
     <tableColumn id="67" xr3:uid="{00000000-0010-0000-0000-000043000000}" name="p_l_sw_post_T2"/>
-    <tableColumn id="69" xr3:uid="{C9E64459-163E-9A4A-9165-7E8C66BCCE69}" name="log_lik"/>
-    <tableColumn id="70" xr3:uid="{BAE2B17A-025A-8D49-9760-390887D490A7}" name="al_win"/>
-    <tableColumn id="71" xr3:uid="{5621703F-F3CE-FF41-9D43-A6AE312C432B}" name="al_loss"/>
-    <tableColumn id="72" xr3:uid="{0B293E2D-F95A-5141-87D7-395B202440AB}" name="kappa"/>
-    <tableColumn id="73" xr3:uid="{79E7B7CC-4CBC-4C48-9548-EBE9CF1427DB}" name="beta_win"/>
-    <tableColumn id="74" xr3:uid="{256345A5-776B-0342-A9BF-B089C9C050C1}" name="beta_loss"/>
+    <tableColumn id="69" xr3:uid="{C9E64459-163E-9A4A-9165-7E8C66BCCE69}" name="al_win"/>
+    <tableColumn id="70" xr3:uid="{BAE2B17A-025A-8D49-9760-390887D490A7}" name="al_loss"/>
+    <tableColumn id="71" xr3:uid="{5621703F-F3CE-FF41-9D43-A6AE312C432B}" name="bet_win"/>
+    <tableColumn id="72" xr3:uid="{0B293E2D-F95A-5141-87D7-395B202440AB}" name="bet_loss"/>
+    <tableColumn id="73" xr3:uid="{79E7B7CC-4CBC-4C48-9548-EBE9CF1427DB}" name="sc_bet_win"/>
+    <tableColumn id="74" xr3:uid="{256345A5-776B-0342-A9BF-B089C9C050C1}" name="sc_bet_loss"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3904,7 +3904,7 @@
   <dimension ref="A1:BV29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="BI1" workbookViewId="0">
-      <selection activeCell="BO11" sqref="BO11"/>
+      <selection activeCell="CA10" sqref="CA10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4121,10 +4121,10 @@
         <v>1148</v>
       </c>
       <c r="BS1" t="s">
+        <v>1149</v>
+      </c>
+      <c r="BT1" t="s">
         <v>1150</v>
-      </c>
-      <c r="BT1" t="s">
-        <v>1149</v>
       </c>
       <c r="BU1" t="s">
         <v>1151</v>
@@ -4339,22 +4339,22 @@
         <v>119</v>
       </c>
       <c r="BQ2">
-        <v>-195.24523001490601</v>
+        <v>3.3749659017537598E-2</v>
       </c>
       <c r="BR2">
-        <v>0.27650000000000002</v>
+        <v>0.34601990922606202</v>
       </c>
       <c r="BS2">
-        <v>0.74339999999999995</v>
+        <v>1.74152919562174</v>
       </c>
       <c r="BT2">
-        <v>-0.59751766350473201</v>
+        <v>0.47967486629865602</v>
       </c>
       <c r="BU2">
-        <v>0.70918673554329703</v>
+        <v>-0.48246735807442798</v>
       </c>
       <c r="BV2">
-        <v>-0.42291431385054601</v>
+        <v>-0.346096577956584</v>
       </c>
     </row>
     <row r="3" spans="1:74" x14ac:dyDescent="0.2">
@@ -4563,22 +4563,22 @@
         <v>101</v>
       </c>
       <c r="BQ3">
-        <v>-165.26080230379301</v>
+        <v>0.22711067812746599</v>
       </c>
       <c r="BR3">
-        <v>0.32290000000000002</v>
+        <v>0.57114357630567403</v>
       </c>
       <c r="BS3">
-        <v>0.88219999999999998</v>
+        <v>1.10546618297845</v>
       </c>
       <c r="BT3">
-        <v>-0.33299572561956597</v>
+        <v>0.54185088284372296</v>
       </c>
       <c r="BU3">
-        <v>1.02957655196939</v>
+        <v>-0.149792832644881</v>
       </c>
       <c r="BV3">
-        <v>0.46879038000710099</v>
+        <v>0.28552077400074899</v>
       </c>
     </row>
     <row r="4" spans="1:74" x14ac:dyDescent="0.2">
@@ -4787,22 +4787,22 @@
         <v>213</v>
       </c>
       <c r="BQ4">
-        <v>-101.47496579892901</v>
+        <v>0.168468865392258</v>
       </c>
       <c r="BR4">
-        <v>0.23</v>
+        <v>0.29856914159399001</v>
       </c>
       <c r="BS4">
-        <v>0.92769999999999997</v>
+        <v>1.46099372204197</v>
       </c>
       <c r="BT4">
-        <v>-1.76299798096754</v>
+        <v>1.0337159556990101</v>
       </c>
       <c r="BU4">
-        <v>1.70106939969715</v>
+        <v>0.13155603791655601</v>
       </c>
       <c r="BV4">
-        <v>1.3525657350028</v>
+        <v>-4.6111333073499003E-2</v>
       </c>
     </row>
     <row r="5" spans="1:74" x14ac:dyDescent="0.2">
@@ -5011,22 +5011,22 @@
         <v>213</v>
       </c>
       <c r="BQ5">
-        <v>-65.755395678022396</v>
+        <v>0.143532833929191</v>
       </c>
       <c r="BR5">
-        <v>0.21859999999999999</v>
+        <v>0.30642130850684601</v>
       </c>
       <c r="BS5">
-        <v>0.61099999999999999</v>
+        <v>1.9133346438900201</v>
       </c>
       <c r="BT5">
-        <v>-0.99090813395190702</v>
+        <v>1.31073622608664</v>
       </c>
       <c r="BU5">
-        <v>2.01221574468331</v>
+        <v>0.141362091414032</v>
       </c>
       <c r="BV5">
-        <v>1.4327477919953999</v>
+        <v>0.50482723298507604</v>
       </c>
     </row>
     <row r="6" spans="1:74" x14ac:dyDescent="0.2">
@@ -5235,22 +5235,22 @@
         <v>305</v>
       </c>
       <c r="BQ6">
-        <v>-193.48568947408901</v>
+        <v>9.0379433712604498E-2</v>
       </c>
       <c r="BR6">
-        <v>0.24859999999999999</v>
+        <v>0.70276377885577701</v>
       </c>
       <c r="BS6">
-        <v>0.92749999999999999</v>
+        <v>0.91939584489317205</v>
       </c>
       <c r="BT6">
-        <v>-0.29302557277204</v>
+        <v>1.02683493665536</v>
       </c>
       <c r="BU6">
-        <v>0.645611501496689</v>
+        <v>0.25227592851584801</v>
       </c>
       <c r="BV6">
-        <v>0.45243428769427402</v>
+        <v>-0.28584661775709702</v>
       </c>
     </row>
     <row r="7" spans="1:74" x14ac:dyDescent="0.2">
@@ -5459,22 +5459,22 @@
         <v>312</v>
       </c>
       <c r="BQ7">
-        <v>-113.570517310347</v>
+        <v>0.108149850154973</v>
       </c>
       <c r="BR7">
-        <v>0.2039</v>
+        <v>0.28373926618510298</v>
       </c>
       <c r="BS7">
-        <v>0.49730000000000002</v>
+        <v>1.84186107435012</v>
       </c>
       <c r="BT7">
-        <v>-0.95623048809300604</v>
+        <v>1.6404560698132</v>
       </c>
       <c r="BU7">
-        <v>1.6559707678286</v>
+        <v>-0.15455867893363101</v>
       </c>
       <c r="BV7">
-        <v>1.6041850537107101</v>
+        <v>0.23331283688676599</v>
       </c>
     </row>
     <row r="8" spans="1:74" x14ac:dyDescent="0.2">
@@ -5680,22 +5680,22 @@
         <v>213</v>
       </c>
       <c r="BQ8">
-        <v>-81.0274810010431</v>
+        <v>0.156593073875155</v>
       </c>
       <c r="BR8">
-        <v>0.29530000000000001</v>
+        <v>0.39302413997605301</v>
       </c>
       <c r="BS8">
-        <v>0.76160000000000005</v>
+        <v>1.9452254807627001</v>
       </c>
       <c r="BT8">
-        <v>-1.22511215610414</v>
+        <v>1.62732142365252</v>
       </c>
       <c r="BU8">
-        <v>1.8751071144323701</v>
+        <v>0.31154256063091901</v>
       </c>
       <c r="BV8">
-        <v>1.3270453347473901</v>
+        <v>-0.40179045698015903</v>
       </c>
     </row>
     <row r="9" spans="1:74" x14ac:dyDescent="0.2">
@@ -5904,22 +5904,22 @@
         <v>437</v>
       </c>
       <c r="BQ9">
-        <v>-153.28737607999301</v>
+        <v>0.29651199330697797</v>
       </c>
       <c r="BR9">
-        <v>0.37509999999999999</v>
+        <v>0.64135026446160803</v>
       </c>
       <c r="BS9">
-        <v>0.87639999999999996</v>
+        <v>0.82787544850094497</v>
       </c>
       <c r="BT9">
-        <v>0.155182060518574</v>
+        <v>0.13453166119818599</v>
       </c>
       <c r="BU9">
-        <v>1.0768682501890099</v>
+        <v>0.72999667581427197</v>
       </c>
       <c r="BV9">
-        <v>5.0772242594244003E-2</v>
+        <v>1.40144688210716</v>
       </c>
     </row>
     <row r="10" spans="1:74" x14ac:dyDescent="0.2">
@@ -6128,22 +6128,22 @@
         <v>213</v>
       </c>
       <c r="BQ10">
-        <v>-36.2772334443777</v>
+        <v>0.107565932900949</v>
       </c>
       <c r="BR10">
-        <v>0.1147</v>
+        <v>0.13500411064186699</v>
       </c>
       <c r="BS10">
-        <v>0.6784</v>
+        <v>2.94487344515893</v>
       </c>
       <c r="BT10">
-        <v>-3.4697156398402198</v>
+        <v>1.6123714771535</v>
       </c>
       <c r="BU10">
-        <v>2.7614574858654</v>
+        <v>0.17348764213457499</v>
       </c>
       <c r="BV10">
-        <v>2.3663676394868398</v>
+        <v>1.2580357289008799</v>
       </c>
     </row>
     <row r="11" spans="1:74" x14ac:dyDescent="0.2">
@@ -6349,22 +6349,22 @@
         <v>334</v>
       </c>
       <c r="BQ11">
-        <v>-176.20970671031299</v>
+        <v>0.197304510781806</v>
       </c>
       <c r="BR11">
-        <v>0.30130000000000001</v>
+        <v>0.28584479782841699</v>
       </c>
       <c r="BS11">
-        <v>0.79469999999999996</v>
+        <v>0.58288409722016599</v>
       </c>
       <c r="BT11">
-        <v>-2.2695774014510102</v>
+        <v>0.52607110064336404</v>
       </c>
       <c r="BU11">
-        <v>0.91615615799420203</v>
+        <v>0.70853159514417996</v>
       </c>
       <c r="BV11">
-        <v>0.72365446505258002</v>
+        <v>0.49921830533690498</v>
       </c>
     </row>
     <row r="12" spans="1:74" x14ac:dyDescent="0.2">
@@ -6573,22 +6573,22 @@
         <v>547</v>
       </c>
       <c r="BQ12">
-        <v>-129.59821727707401</v>
+        <v>0.443162596624875</v>
       </c>
       <c r="BR12">
-        <v>0.47770000000000001</v>
+        <v>0.51995011929615098</v>
       </c>
       <c r="BS12">
-        <v>0.90669999999999995</v>
+        <v>1.13982551054293</v>
       </c>
       <c r="BT12">
-        <v>-0.31101176545220599</v>
+        <v>0.99202346820181997</v>
       </c>
       <c r="BU12">
-        <v>1.1192423119757899</v>
+        <v>-0.15846268473448699</v>
       </c>
       <c r="BV12">
-        <v>1.03779990004914</v>
+        <v>0.16787458272271299</v>
       </c>
     </row>
     <row r="13" spans="1:74" x14ac:dyDescent="0.2">
@@ -6797,22 +6797,22 @@
         <v>213</v>
       </c>
       <c r="BQ13">
-        <v>-60.571385672718101</v>
+        <v>0.215528105305304</v>
       </c>
       <c r="BR13">
-        <v>0.31480000000000002</v>
+        <v>0.30652054875453399</v>
       </c>
       <c r="BS13">
-        <v>0.61270000000000002</v>
+        <v>2.1839780414740102</v>
       </c>
       <c r="BT13">
-        <v>-1.32791011237045</v>
+        <v>1.94047625893135</v>
       </c>
       <c r="BU13">
-        <v>2.0580095457991399</v>
+        <v>-6.0761536405578402E-2</v>
       </c>
       <c r="BV13">
-        <v>1.43560488757254</v>
+        <v>-0.81953891198047701</v>
       </c>
     </row>
     <row r="14" spans="1:74" x14ac:dyDescent="0.2">
@@ -7021,22 +7021,22 @@
         <v>213</v>
       </c>
       <c r="BQ14">
-        <v>-94.976580414405802</v>
+        <v>0.45457115321685698</v>
       </c>
       <c r="BR14">
-        <v>0.42920000000000003</v>
+        <v>0.50571942681840698</v>
       </c>
       <c r="BS14">
-        <v>0.92079999999999995</v>
+        <v>1.35335469809391</v>
       </c>
       <c r="BT14">
-        <v>-0.43466934283172798</v>
+        <v>0.75650556699043503</v>
       </c>
       <c r="BU14">
-        <v>1.5280735742400799</v>
+        <v>0.17011508376602</v>
       </c>
       <c r="BV14">
-        <v>0.80703860568608998</v>
+        <v>0.37579360453347299</v>
       </c>
     </row>
     <row r="15" spans="1:74" x14ac:dyDescent="0.2">
@@ -7245,22 +7245,22 @@
         <v>661</v>
       </c>
       <c r="BQ15">
-        <v>-105.125024479212</v>
+        <v>0.373434423478611</v>
       </c>
       <c r="BR15">
-        <v>0.41760000000000003</v>
+        <v>0.460098826390475</v>
       </c>
       <c r="BS15">
-        <v>0.82040000000000002</v>
+        <v>1.5306011420310599</v>
       </c>
       <c r="BT15">
-        <v>-0.73835003836202995</v>
+        <v>0.56547843668977704</v>
       </c>
       <c r="BU15">
-        <v>1.6033147288251199</v>
+        <v>7.8578762001784805E-2</v>
       </c>
       <c r="BV15">
-        <v>8.2613650931698895E-2</v>
+        <v>-0.84655485837810596</v>
       </c>
     </row>
     <row r="16" spans="1:74" x14ac:dyDescent="0.2">
@@ -7469,22 +7469,22 @@
         <v>213</v>
       </c>
       <c r="BQ16">
-        <v>-57.811669798091401</v>
+        <v>0.19604022275664701</v>
       </c>
       <c r="BR16">
-        <v>0.30570000000000003</v>
+        <v>0.35035087748668298</v>
       </c>
       <c r="BS16">
-        <v>0.76500000000000001</v>
+        <v>2.3922539209142499</v>
       </c>
       <c r="BT16">
-        <v>-1.47391208041934</v>
+        <v>1.88571675302126</v>
       </c>
       <c r="BU16">
-        <v>2.09398730181656</v>
+        <v>-0.27389114201592901</v>
       </c>
       <c r="BV16">
-        <v>1.75676989537803</v>
+        <v>-0.35290988002387302</v>
       </c>
     </row>
     <row r="17" spans="1:74" x14ac:dyDescent="0.2">
@@ -7693,22 +7693,22 @@
         <v>245</v>
       </c>
       <c r="BQ17">
-        <v>-115.194053235957</v>
+        <v>0.10209777107449899</v>
       </c>
       <c r="BR17">
-        <v>0.26200000000000001</v>
+        <v>0.38112066674259498</v>
       </c>
       <c r="BS17">
-        <v>0.82210000000000005</v>
+        <v>1.68348988229774</v>
       </c>
       <c r="BT17">
-        <v>-1.0707873426015899</v>
+        <v>0.93049963251203904</v>
       </c>
       <c r="BU17">
-        <v>1.5906079169978899</v>
+        <v>0.23762322213363499</v>
       </c>
       <c r="BV17">
-        <v>0.69118923646263297</v>
+        <v>4.98494571118904E-2</v>
       </c>
     </row>
     <row r="18" spans="1:74" x14ac:dyDescent="0.2">
@@ -7914,22 +7914,22 @@
         <v>126</v>
       </c>
       <c r="BQ18">
-        <v>-100.150514235363</v>
+        <v>0.188924251774887</v>
       </c>
       <c r="BR18">
-        <v>0.31340000000000001</v>
+        <v>0.66270029189331303</v>
       </c>
       <c r="BS18">
-        <v>0.89759999999999995</v>
+        <v>1.6210445900649</v>
       </c>
       <c r="BT18">
-        <v>0.369544565129868</v>
+        <v>1.2784920597824001</v>
       </c>
       <c r="BU18">
-        <v>1.5011309256635199</v>
+        <v>0.14197864775852201</v>
       </c>
       <c r="BV18">
-        <v>0.99966629456970302</v>
+        <v>-0.13141936209968499</v>
       </c>
     </row>
     <row r="19" spans="1:74" x14ac:dyDescent="0.2">
@@ -8135,22 +8135,22 @@
         <v>101</v>
       </c>
       <c r="BQ19">
-        <v>-176.71758865828599</v>
+        <v>1.47408103222445E-2</v>
       </c>
       <c r="BR19">
-        <v>0.1067</v>
+        <v>0.100391849746247</v>
       </c>
       <c r="BS19">
-        <v>0.72709999999999997</v>
+        <v>2.1119107178987999</v>
       </c>
       <c r="BT19">
-        <v>-1.2759578059546901</v>
+        <v>0.87684533040774404</v>
       </c>
       <c r="BU19">
-        <v>1.4511630742980901</v>
+        <v>-0.13404313871812601</v>
       </c>
       <c r="BV19">
-        <v>-5.4760836326000199E-2</v>
+        <v>-0.38127798850820399</v>
       </c>
     </row>
     <row r="20" spans="1:74" x14ac:dyDescent="0.2">
@@ -8359,22 +8359,22 @@
         <v>836</v>
       </c>
       <c r="BQ20">
-        <v>-101.67088325247801</v>
+        <v>0.241294417481065</v>
       </c>
       <c r="BR20">
-        <v>0.317</v>
+        <v>0.43362811489248598</v>
       </c>
       <c r="BS20">
-        <v>0.81130000000000002</v>
+        <v>2.12083714768929</v>
       </c>
       <c r="BT20">
-        <v>-0.54412988590080202</v>
+        <v>1.2602974438961401</v>
       </c>
       <c r="BU20">
-        <v>1.7790091285483101</v>
+        <v>-0.480528276238676</v>
       </c>
       <c r="BV20">
-        <v>1.12841757442276</v>
+        <v>-0.19015492769551801</v>
       </c>
     </row>
     <row r="21" spans="1:74" x14ac:dyDescent="0.2">
@@ -8583,22 +8583,22 @@
         <v>99</v>
       </c>
       <c r="BQ21">
-        <v>-134.796221624216</v>
+        <v>0.33289019028123701</v>
       </c>
       <c r="BR21">
-        <v>0.36940000000000001</v>
+        <v>0.442045457138729</v>
       </c>
       <c r="BS21">
-        <v>0.89710000000000001</v>
+        <v>1.1537117661419101</v>
       </c>
       <c r="BT21">
-        <v>-1.1831840361529</v>
+        <v>0.54437650501970403</v>
       </c>
       <c r="BU21">
-        <v>1.3234407918386299</v>
+        <v>0.13735357715461599</v>
       </c>
       <c r="BV21">
-        <v>0.482531567602069</v>
+        <v>-0.30504896353712202</v>
       </c>
     </row>
     <row r="22" spans="1:74" x14ac:dyDescent="0.2">
@@ -8807,22 +8807,22 @@
         <v>196</v>
       </c>
       <c r="BQ22">
-        <v>-98.593096553727406</v>
+        <v>0.20564889429056299</v>
       </c>
       <c r="BR22">
-        <v>0.26889999999999997</v>
+        <v>0.40186403845827301</v>
       </c>
       <c r="BS22">
-        <v>0.87370000000000003</v>
+        <v>1.79293778213238</v>
       </c>
       <c r="BT22">
-        <v>-1.2795619426334099</v>
+        <v>1.43303948217488</v>
       </c>
       <c r="BU22">
-        <v>1.8796881403993599</v>
+        <v>7.9673160204535201E-2</v>
       </c>
       <c r="BV22">
-        <v>0.82152876434571698</v>
+        <v>-0.97505363676711299</v>
       </c>
     </row>
     <row r="23" spans="1:74" x14ac:dyDescent="0.2">
@@ -9031,22 +9031,22 @@
         <v>213</v>
       </c>
       <c r="BQ23">
-        <v>-117.579142180875</v>
+        <v>0.214718034975173</v>
       </c>
       <c r="BR23">
-        <v>0.32040000000000002</v>
+        <v>0.44823018226292399</v>
       </c>
       <c r="BS23">
-        <v>0.86150000000000004</v>
+        <v>1.7953024570010201</v>
       </c>
       <c r="BT23">
-        <v>-0.71704458688894102</v>
+        <v>1.06712222423887</v>
       </c>
       <c r="BU23">
-        <v>1.4631170900794599</v>
+        <v>-0.53540111260789902</v>
       </c>
       <c r="BV23">
-        <v>1.08708767510257</v>
+        <v>0.31007950480854701</v>
       </c>
     </row>
     <row r="24" spans="1:74" x14ac:dyDescent="0.2">
@@ -9255,22 +9255,22 @@
         <v>330</v>
       </c>
       <c r="BQ24">
-        <v>-162.18186632209</v>
+        <v>4.2428203848660098E-2</v>
       </c>
       <c r="BR24">
-        <v>0.12759999999999999</v>
+        <v>6.3980076271133099E-2</v>
       </c>
       <c r="BS24">
-        <v>0.25459999999999999</v>
+        <v>1.83228156649898</v>
       </c>
       <c r="BT24">
-        <v>-2.0520179673243502</v>
+        <v>1.7934711077149701</v>
       </c>
       <c r="BU24">
-        <v>1.5873608032834201</v>
+        <v>3.7947630266227002E-2</v>
       </c>
       <c r="BV24">
-        <v>0.96186727280885898</v>
+        <v>-0.77441235839064204</v>
       </c>
     </row>
     <row r="25" spans="1:74" x14ac:dyDescent="0.2">
@@ -9479,22 +9479,22 @@
         <v>95</v>
       </c>
       <c r="BQ25">
-        <v>-58.184112111257299</v>
+        <v>0.20403438305475999</v>
       </c>
       <c r="BR25">
-        <v>0.30249999999999999</v>
+        <v>0.23610185335377301</v>
       </c>
       <c r="BS25">
-        <v>0.50680000000000003</v>
+        <v>2.0239735182112102</v>
       </c>
       <c r="BT25">
-        <v>-1.0714361175579501</v>
+        <v>2.3314785751660398</v>
       </c>
       <c r="BU25">
-        <v>1.8317257290739599</v>
+        <v>-0.20121067857813299</v>
       </c>
       <c r="BV25">
-        <v>1.8052383920493</v>
+        <v>-0.68347323761426704</v>
       </c>
     </row>
     <row r="26" spans="1:74" x14ac:dyDescent="0.2">
@@ -9703,22 +9703,22 @@
         <v>713</v>
       </c>
       <c r="BQ26">
-        <v>-75.349284475398306</v>
+        <v>0.140533382413114</v>
       </c>
       <c r="BR26">
-        <v>0.33450000000000002</v>
+        <v>0.221742667078277</v>
       </c>
       <c r="BS26">
-        <v>0.32969999999999999</v>
+        <v>1.84442343638814</v>
       </c>
       <c r="BT26">
-        <v>-1.5480920879250499</v>
+        <v>2.3879442920877598</v>
       </c>
       <c r="BU26">
-        <v>1.71137806116449</v>
+        <v>-6.2232260737934003E-2</v>
       </c>
       <c r="BV26">
-        <v>2.2558751583223802</v>
+        <v>-0.32530782700728</v>
       </c>
     </row>
     <row r="27" spans="1:74" x14ac:dyDescent="0.2">
@@ -9927,22 +9927,22 @@
         <v>843</v>
       </c>
       <c r="BQ27">
-        <v>-114.67111241329999</v>
+        <v>0.23282562272131299</v>
       </c>
       <c r="BR27">
-        <v>0.32540000000000002</v>
+        <v>0.65056803878946301</v>
       </c>
       <c r="BS27">
-        <v>0.89729999999999999</v>
+        <v>1.7782001530629601</v>
       </c>
       <c r="BT27">
-        <v>-0.81103065015539</v>
+        <v>0.51214732272857799</v>
       </c>
       <c r="BU27">
-        <v>1.70783692537763</v>
+        <v>-0.17559169365990401</v>
       </c>
       <c r="BV27">
-        <v>-0.125085432174869</v>
+        <v>-0.72686406206242404</v>
       </c>
     </row>
     <row r="28" spans="1:74" x14ac:dyDescent="0.2">
@@ -10151,22 +10151,22 @@
         <v>126</v>
       </c>
       <c r="BQ28">
-        <v>-49.3868939940239</v>
+        <v>0.16351552882031301</v>
       </c>
       <c r="BR28">
-        <v>0.27060000000000001</v>
+        <v>0.214621949934555</v>
       </c>
       <c r="BS28">
-        <v>0.72709999999999997</v>
+        <v>2.8685449948128801</v>
       </c>
       <c r="BT28">
-        <v>-2.0177914044123502</v>
+        <v>1.62059239386302</v>
       </c>
       <c r="BU28">
-        <v>2.4039996018230299</v>
+        <v>0.10024782188338099</v>
       </c>
       <c r="BV28">
-        <v>1.8365387948684899</v>
+        <v>0.35687285947530001</v>
       </c>
     </row>
     <row r="29" spans="1:74" x14ac:dyDescent="0.2">
@@ -10375,22 +10375,22 @@
         <v>647</v>
       </c>
       <c r="BQ29">
-        <v>-82.294699015430794</v>
+        <v>7.0548161359247699E-2</v>
       </c>
       <c r="BR29">
-        <v>0.19639999999999999</v>
+        <v>0.22567393990067999</v>
       </c>
       <c r="BS29">
-        <v>0.23749999999999999</v>
+        <v>2.1874361525966601</v>
       </c>
       <c r="BT29">
-        <v>-0.36222088391919599</v>
+        <v>1.8522920520388799</v>
       </c>
       <c r="BU29">
-        <v>1.96481284620143</v>
+        <v>0.45147420617223999</v>
       </c>
       <c r="BV29">
-        <v>1.6009380656563701</v>
+        <v>0.13403400562437701</v>
       </c>
     </row>
   </sheetData>

</xml_diff>